<commit_message>
Add messy header challenge data
</commit_message>
<xml_diff>
--- a/data/read_challenge/metadata_and_messy_header.xlsx
+++ b/data/read_challenge/metadata_and_messy_header.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selina\Repos\Work\intro-r-data-analysis\data\read_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{266D2724-F12B-4894-ABCF-0B6D8DFE1F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A81EF5-33D0-40B8-B37F-14BE4284DD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21330" yWindow="5865" windowWidth="19755" windowHeight="19215" activeTab="1" xr2:uid="{9470E1A0-FE24-45D0-9A1A-4360F96A49D4}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{9470E1A0-FE24-45D0-9A1A-4360F96A49D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t># Study: Insect Biodiversity in Urban Parks</t>
   </si>
@@ -48,9 +48,6 @@
     <t># Date: 2025-02-20</t>
   </si>
   <si>
-    <t xml:space="preserve">Species Name </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Count@</t>
   </si>
   <si>
@@ -66,13 +63,13 @@
     <t>Apis mellifera</t>
   </si>
   <si>
-    <t xml:space="preserve">  75.2</t>
-  </si>
-  <si>
     <t>Vespula vulgaris</t>
   </si>
   <si>
     <t xml:space="preserve">  60.1</t>
+  </si>
+  <si>
+    <t>Species Name °C</t>
   </si>
 </sst>
 </file>
@@ -447,7 +444,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B71A96B-05B9-474D-B589-65DE912CE63E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,46 +499,43 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>